<commit_message>
actualizacion de registros con hash
</commit_message>
<xml_diff>
--- a/output/Bienes/Bienes_03_CONTRATOS.xlsx
+++ b/output/Bienes/Bienes_03_CONTRATOS.xlsx
@@ -3261,7 +3261,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -8931,7 +8931,7 @@
       </c>
       <c r="J135" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K135" t="inlineStr">
@@ -18507,7 +18507,7 @@
       </c>
       <c r="J287" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K287" t="inlineStr">
@@ -18633,7 +18633,7 @@
       </c>
       <c r="J289" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K289" t="inlineStr">
@@ -18696,7 +18696,7 @@
       </c>
       <c r="J290" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K290" t="inlineStr">
@@ -18759,7 +18759,7 @@
       </c>
       <c r="J291" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K291" t="inlineStr">
@@ -18822,7 +18822,7 @@
       </c>
       <c r="J292" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K292" t="inlineStr">
@@ -18885,7 +18885,7 @@
       </c>
       <c r="J293" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K293" t="inlineStr">
@@ -19326,7 +19326,7 @@
       </c>
       <c r="J300" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K300" t="inlineStr">
@@ -19389,7 +19389,7 @@
       </c>
       <c r="J301" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K301" t="inlineStr">
@@ -19452,7 +19452,7 @@
       </c>
       <c r="J302" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K302" t="inlineStr">
@@ -19515,7 +19515,7 @@
       </c>
       <c r="J303" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K303" t="inlineStr">
@@ -19578,7 +19578,7 @@
       </c>
       <c r="J304" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K304" t="inlineStr">
@@ -19641,7 +19641,7 @@
       </c>
       <c r="J305" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K305" t="inlineStr">
@@ -19704,7 +19704,7 @@
       </c>
       <c r="J306" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K306" t="inlineStr">
@@ -19767,7 +19767,7 @@
       </c>
       <c r="J307" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K307" t="inlineStr">
@@ -19830,7 +19830,7 @@
       </c>
       <c r="J308" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K308" t="inlineStr">
@@ -19956,7 +19956,7 @@
       </c>
       <c r="J310" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K310" t="inlineStr">
@@ -20019,7 +20019,7 @@
       </c>
       <c r="J311" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K311" t="inlineStr">
@@ -20082,7 +20082,7 @@
       </c>
       <c r="J312" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K312" t="inlineStr">
@@ -20145,7 +20145,7 @@
       </c>
       <c r="J313" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K313" t="inlineStr">
@@ -20208,7 +20208,7 @@
       </c>
       <c r="J314" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K314" t="inlineStr">
@@ -20271,7 +20271,7 @@
       </c>
       <c r="J315" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K315" t="inlineStr">
@@ -20334,7 +20334,7 @@
       </c>
       <c r="J316" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K316" t="inlineStr">
@@ -20397,7 +20397,7 @@
       </c>
       <c r="J317" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K317" t="inlineStr">
@@ -20460,7 +20460,7 @@
       </c>
       <c r="J318" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K318" t="inlineStr">
@@ -20523,7 +20523,7 @@
       </c>
       <c r="J319" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K319" t="inlineStr">
@@ -20586,7 +20586,7 @@
       </c>
       <c r="J320" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K320" t="inlineStr">
@@ -20649,7 +20649,7 @@
       </c>
       <c r="J321" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K321" t="inlineStr">
@@ -20712,7 +20712,7 @@
       </c>
       <c r="J322" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K322" t="inlineStr">
@@ -20775,7 +20775,7 @@
       </c>
       <c r="J323" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K323" t="inlineStr">
@@ -20901,7 +20901,7 @@
       </c>
       <c r="J325" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K325" t="inlineStr">
@@ -20964,7 +20964,7 @@
       </c>
       <c r="J326" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K326" t="inlineStr">
@@ -21027,7 +21027,7 @@
       </c>
       <c r="J327" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K327" t="inlineStr">
@@ -21090,7 +21090,7 @@
       </c>
       <c r="J328" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K328" t="inlineStr">
@@ -21153,7 +21153,7 @@
       </c>
       <c r="J329" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K329" t="inlineStr">
@@ -21216,7 +21216,7 @@
       </c>
       <c r="J330" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K330" t="inlineStr">
@@ -21279,7 +21279,7 @@
       </c>
       <c r="J331" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K331" t="inlineStr">
@@ -21342,7 +21342,7 @@
       </c>
       <c r="J332" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K332" t="inlineStr">
@@ -21468,7 +21468,7 @@
       </c>
       <c r="J334" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K334" t="inlineStr">
@@ -21531,7 +21531,7 @@
       </c>
       <c r="J335" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K335" t="inlineStr">
@@ -21594,7 +21594,7 @@
       </c>
       <c r="J336" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K336" t="inlineStr">
@@ -21657,7 +21657,7 @@
       </c>
       <c r="J337" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K337" t="inlineStr">
@@ -22350,7 +22350,7 @@
       </c>
       <c r="J348" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K348" t="inlineStr">

</xml_diff>